<commit_message>
Updated some doc files
</commit_message>
<xml_diff>
--- a/docs/Arbeitszeit_Topeiner.xlsx
+++ b/docs/Arbeitszeit_Topeiner.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DiplomarbeitFileSharing\stream\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846AB557-DF68-4728-83FD-ED02F8DA54E1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C18055-2CD0-4461-B78D-9AF1A7A59D57}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,10 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Diplomarbeit "Filesharing with BitTorrent</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Arbeitszeit Topeiner</t>
   </si>
@@ -39,30 +36,65 @@
     <t>Datum</t>
   </si>
   <si>
-    <t>Zeit</t>
-  </si>
-  <si>
     <t>Arbeit</t>
   </si>
   <si>
-    <t>1 h</t>
-  </si>
-  <si>
     <t>Einlesen in das Thema, Arbeiten an Konzept</t>
   </si>
   <si>
-    <t>1h</t>
-  </si>
-  <si>
     <t>Einlesen in das Thema, Aktualisierung des Repositorys</t>
+  </si>
+  <si>
+    <t>Recherche zum Einbinden externer Bibliotheken ins Projekt (Github), Ergänzungen in DiplomarbeitsDB</t>
+  </si>
+  <si>
+    <t>Einführung in die DiplomarbeitsDB</t>
+  </si>
+  <si>
+    <t>Erstes Konzept für UI entwicklen</t>
+  </si>
+  <si>
+    <t>Weiterarbeiten an UI-Konzept, Recherche zum Einbinden von MaterialUI in Java-Projekte</t>
+  </si>
+  <si>
+    <t>Fertigstellen des UI-Konzepts</t>
+  </si>
+  <si>
+    <t>Diplomarbeit "stream - Filesharing with BitTorrent"</t>
+  </si>
+  <si>
+    <t>Statusupdate erstellt</t>
+  </si>
+  <si>
+    <t>Arbeiten am Github-Repository, Grundlegenden Code erstellt, Ergänzungen in Trello</t>
+  </si>
+  <si>
+    <t>Zeit in h</t>
+  </si>
+  <si>
+    <t>Erforderlicher Arbeitsaufwand in h</t>
+  </si>
+  <si>
+    <t>Aktueller Arbeitsaufwand in h</t>
+  </si>
+  <si>
+    <t>Aktualisierung einiger doc files, Einlesen in spiegeln von Repositories</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -78,7 +110,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -86,13 +118,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -407,64 +467,177 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" customWidth="1"/>
-    <col min="4" max="4" width="43" customWidth="1"/>
+    <col min="1" max="1" width="44.6640625" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" style="2" customWidth="1"/>
+    <col min="3" max="4" width="17.109375" style="8" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="15.21875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="89" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="8">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="8">
+        <f>SUM(F:F)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E7" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+      <c r="F7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E8" s="3">
+        <v>43492</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E9" s="3">
+        <v>43523</v>
+      </c>
+      <c r="F9" s="4">
+        <v>1</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B5" s="1">
-        <v>43492</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E10" s="3">
+        <v>43647</v>
+      </c>
+      <c r="F10" s="4">
+        <v>1</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E11" s="3">
+        <v>43650</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E12" s="3">
+        <v>43661</v>
+      </c>
+      <c r="F12" s="4">
+        <v>2</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="1">
-        <v>43523</v>
-      </c>
-      <c r="C6" t="s">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E13" s="3">
+        <v>43662</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E14" s="3">
+        <v>43665</v>
+      </c>
+      <c r="F14" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D6" t="s">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E15" s="3">
+        <v>43666</v>
+      </c>
+      <c r="F15" s="4">
+        <v>1</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E16" s="3">
+        <v>43669</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E17" s="3">
+        <v>43670</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Created three UI versions, updated document Arbeitszeit_Topeiner
</commit_message>
<xml_diff>
--- a/docs/Arbeitszeit_Topeiner.xlsx
+++ b/docs/Arbeitszeit_Topeiner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DiplomarbeitFileSharing\stream\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C18055-2CD0-4461-B78D-9AF1A7A59D57}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E29559-111D-4346-B76D-27F4ACA83F1D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Arbeitszeit Topeiner</t>
   </si>
@@ -79,6 +79,15 @@
   </si>
   <si>
     <t>Aktualisierung einiger doc files, Einlesen in spiegeln von Repositories</t>
+  </si>
+  <si>
+    <t>Anregungen für die Erstellung einer UI gesucht</t>
+  </si>
+  <si>
+    <t>Erstellung einer ersten UI mit SceneBuilder</t>
+  </si>
+  <si>
+    <t>Weitere UI-Designs mit SceneBuilder erstellt, insgesamt 3 Designs fertiggestellt, Statusupdate gegeben</t>
   </si>
 </sst>
 </file>
@@ -467,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -512,7 +521,7 @@
       </c>
       <c r="C5" s="8">
         <f>SUM(F:F)</f>
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -634,6 +643,39 @@
       </c>
       <c r="G17" s="5" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E18" s="3">
+        <v>43671</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E19" s="3">
+        <v>43674</v>
+      </c>
+      <c r="F19" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E20" s="3">
+        <v>43675</v>
+      </c>
+      <c r="F20" s="4">
+        <v>2</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked on stream-UI, updated Arbeitszeit_Topeiner
</commit_message>
<xml_diff>
--- a/docs/Arbeitszeit_Topeiner.xlsx
+++ b/docs/Arbeitszeit_Topeiner.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DiplomarbeitFileSharing\stream\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E29559-111D-4346-B76D-27F4ACA83F1D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B6E1B7-1158-4380-AF7C-8509BEFD9A35}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Arbeitszeit Topeiner</t>
   </si>
@@ -88,6 +88,17 @@
   </si>
   <si>
     <t>Weitere UI-Designs mit SceneBuilder erstellt, insgesamt 3 Designs fertiggestellt, Statusupdate gegeben</t>
+  </si>
+  <si>
+    <t>Arbeiten am ausgewählten Design (UI resizeable machen)</t>
+  </si>
+  <si>
+    <t>Probleme beim Arbeiten an der UI aufgetreten (UI ist aufgrund des Designs nicht so leicht resizeable zu machen,
+wäre mit höheren Arbeitsaufwand verbunden), Arbeiten an dieser Funktion auf späteren Zeitpunkt verschoben
+Optische Anpassungen an Design</t>
+  </si>
+  <si>
+    <t>Funktionalität der UI programmiert</t>
   </si>
 </sst>
 </file>
@@ -140,7 +151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -161,6 +172,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -476,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -489,7 +503,7 @@
     <col min="3" max="4" width="17.109375" style="8" customWidth="1"/>
     <col min="5" max="5" width="16.44140625" style="4" customWidth="1"/>
     <col min="6" max="6" width="15.21875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="89" style="5" customWidth="1"/>
+    <col min="7" max="7" width="91.77734375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -521,7 +535,7 @@
       </c>
       <c r="C5" s="8">
         <f>SUM(F:F)</f>
-        <v>15</v>
+        <v>21.75</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -650,7 +664,7 @@
         <v>43671</v>
       </c>
       <c r="F18" s="4">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>17</v>
@@ -672,10 +686,37 @@
         <v>43675</v>
       </c>
       <c r="F20" s="4">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E21" s="3">
+        <v>43683</v>
+      </c>
+      <c r="F21" s="4">
+        <v>2</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="5:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="E22" s="3">
+        <v>43684</v>
+      </c>
+      <c r="F22" s="4">
+        <v>4</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="G23" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked on stream-UI (updated menu) Updated Arbeitszeit_Topeiner
</commit_message>
<xml_diff>
--- a/docs/Arbeitszeit_Topeiner.xlsx
+++ b/docs/Arbeitszeit_Topeiner.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DiplomarbeitFileSharing\stream\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B6E1B7-1158-4380-AF7C-8509BEFD9A35}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916889AA-C40A-4B34-B202-456E0E2DB634}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>Arbeitszeit Topeiner</t>
   </si>
@@ -99,6 +99,18 @@
   </si>
   <si>
     <t>Funktionalität der UI programmiert</t>
+  </si>
+  <si>
+    <t>Funktionalität der UI programmiert, Probleme beim Zuweisen von Eigenschaften im Scene Builder</t>
+  </si>
+  <si>
+    <t>Fehlersuche in Scene Builder</t>
+  </si>
+  <si>
+    <t>Aufbau der UI überdacht, neuer Menüpunkt eingefügt</t>
+  </si>
+  <si>
+    <t>Neuer Menüpunkt eingefügt</t>
   </si>
 </sst>
 </file>
@@ -490,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -535,7 +547,7 @@
       </c>
       <c r="C5" s="8">
         <f>SUM(F:F)</f>
-        <v>21.75</v>
+        <v>31.45</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -715,7 +727,112 @@
       </c>
     </row>
     <row r="23" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E23" s="3">
+        <v>43685</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0.5</v>
+      </c>
       <c r="G23" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E24" s="3">
+        <v>43689</v>
+      </c>
+      <c r="F24" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E25" s="3">
+        <v>43690</v>
+      </c>
+      <c r="F25" s="4">
+        <v>1</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E26" s="3">
+        <v>43692</v>
+      </c>
+      <c r="F26" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E27" s="3">
+        <v>43695</v>
+      </c>
+      <c r="F27" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E28" s="3">
+        <v>43699</v>
+      </c>
+      <c r="F28" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E29" s="3">
+        <v>43700</v>
+      </c>
+      <c r="F29" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E30" s="3">
+        <v>43705</v>
+      </c>
+      <c r="F30" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E31" s="3">
+        <v>43711</v>
+      </c>
+      <c r="F31" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E32" s="3">
+        <v>43712</v>
+      </c>
+      <c r="F32" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="G32" s="5" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Worked on stream-UI (changed structure and language of the application) implemented slogan "share better"
</commit_message>
<xml_diff>
--- a/docs/Arbeitszeit_Topeiner.xlsx
+++ b/docs/Arbeitszeit_Topeiner.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DiplomarbeitFileSharing\stream\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916889AA-C40A-4B34-B202-456E0E2DB634}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F3C84C-B786-4AF4-91D7-83DAF4CB1EA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>Arbeitszeit Topeiner</t>
   </si>
@@ -111,6 +111,36 @@
   </si>
   <si>
     <t>Neuer Menüpunkt eingefügt</t>
+  </si>
+  <si>
+    <t>Kurzes Team-Meeting</t>
+  </si>
+  <si>
+    <t>Team-Meeting</t>
+  </si>
+  <si>
+    <t>Pflichtenheft erstellt, Termine und andere Informationen für die Diplomarbeit erhalten</t>
+  </si>
+  <si>
+    <t>Projektplan mit MS Project erstellt</t>
+  </si>
+  <si>
+    <t>Projektplan mit Informationen meines Kollegen ergänzt und fertiggestellt</t>
+  </si>
+  <si>
+    <t>Pflichtenheft ergänzt</t>
+  </si>
+  <si>
+    <t>Pflichtenheft fertiggestellt, Arbeiten an UI</t>
+  </si>
+  <si>
+    <t>Diplomarbeitspräsentation erstellt</t>
+  </si>
+  <si>
+    <t>Anpassungen an der UI vorgenommen (Aufbau der Funktion "Hinzufügen eines Torrents" verändert), Logo implementiert</t>
+  </si>
+  <si>
+    <t>Sprache der UI geändert, Icon erstellt und eingebunden</t>
   </si>
 </sst>
 </file>
@@ -502,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -547,7 +577,7 @@
       </c>
       <c r="C5" s="8">
         <f>SUM(F:F)</f>
-        <v>31.45</v>
+        <v>51.45</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -834,6 +864,149 @@
       </c>
       <c r="G32" s="5" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E33" s="3">
+        <v>43716</v>
+      </c>
+      <c r="F33" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E34" s="3">
+        <v>43717</v>
+      </c>
+      <c r="F34" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E35" s="3">
+        <v>43718</v>
+      </c>
+      <c r="F35" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E36" s="3">
+        <v>43719</v>
+      </c>
+      <c r="F36" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E37" s="3">
+        <v>43721</v>
+      </c>
+      <c r="F37" s="4">
+        <v>4</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E38" s="3">
+        <v>43724</v>
+      </c>
+      <c r="F38" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E39" s="3">
+        <v>43726</v>
+      </c>
+      <c r="F39" s="4">
+        <v>1</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E40" s="3">
+        <v>43732</v>
+      </c>
+      <c r="F40" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E41" s="3">
+        <v>43734</v>
+      </c>
+      <c r="F41" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E42" s="3">
+        <v>43735</v>
+      </c>
+      <c r="F42" s="4">
+        <v>4</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E43" s="3">
+        <v>43738</v>
+      </c>
+      <c r="F43" s="4">
+        <v>2</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E44" s="3">
+        <v>43758</v>
+      </c>
+      <c r="F44" s="4">
+        <v>4</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E45" s="3">
+        <v>43759</v>
+      </c>
+      <c r="F45" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked on stream UI - replaced awt filedialog with javafx filedialog - updated menu entries Updated Arbeitszeit_Topeiner
</commit_message>
<xml_diff>
--- a/docs/Arbeitszeit_Topeiner.xlsx
+++ b/docs/Arbeitszeit_Topeiner.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DiplomarbeitFileSharing\stream\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F3C84C-B786-4AF4-91D7-83DAF4CB1EA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8A74F5-8886-4B99-95FB-0B0EC723848F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
   <si>
     <t>Arbeitszeit Topeiner</t>
   </si>
@@ -140,7 +142,32 @@
     <t>Anpassungen an der UI vorgenommen (Aufbau der Funktion "Hinzufügen eines Torrents" verändert), Logo implementiert</t>
   </si>
   <si>
-    <t>Sprache der UI geändert, Icon erstellt und eingebunden</t>
+    <t>Statusupdate erstellt, Sprache der UI geändert, Icon erstellt und eingebunden</t>
+  </si>
+  <si>
+    <t>Diplomarbeitspräsentation Titelblattdesign bearbeitet</t>
+  </si>
+  <si>
+    <t>Diplomarbeitspräsentation bearbeitet</t>
+  </si>
+  <si>
+    <t>Recherche zum Ändern der Sprache während der Laufzeit</t>
+  </si>
+  <si>
+    <t>Tests zum Ändern der Sprache während der Laufzeit</t>
+  </si>
+  <si>
+    <t>Anmeldung zu den Wettbewerben "Technik fürs Leben Preis Bosch" und "Jugend Innovativ Preis"</t>
+  </si>
+  <si>
+    <t>Änderungen am Design der Diplomarbeitspräsentation</t>
+  </si>
+  <si>
+    <t>Änderungen an UI (unter Menüpunkt 'Add Torrent')</t>
+  </si>
+  <si>
+    <t>Team-Meeting mit Betreuungslehrer, Noch ausstehende Funktionen überdacht und ausgemacht
+(--&gt; resizeable, FileChooser, ResourceBundles, …)</t>
   </si>
 </sst>
 </file>
@@ -532,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+    <sheetView tabSelected="1" topLeftCell="B46" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -577,7 +604,7 @@
       </c>
       <c r="C5" s="8">
         <f>SUM(F:F)</f>
-        <v>51.45</v>
+        <v>72.45</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1003,10 +1030,120 @@
         <v>43759</v>
       </c>
       <c r="F45" s="4">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E46" s="3">
+        <v>43766</v>
+      </c>
+      <c r="F46" s="4">
+        <v>2</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E47" s="3">
+        <v>43767</v>
+      </c>
+      <c r="F47" s="4">
+        <v>2</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="48" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E48" s="3">
+        <v>43773</v>
+      </c>
+      <c r="F48" s="4">
+        <v>2</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E49" s="3">
+        <v>43774</v>
+      </c>
+      <c r="F49" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E50" s="3">
+        <v>43780</v>
+      </c>
+      <c r="F50" s="4">
+        <v>4</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="51" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E51" s="3">
+        <v>43787</v>
+      </c>
+      <c r="F51" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="52" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E52" s="3">
+        <v>43794</v>
+      </c>
+      <c r="F52" s="4">
+        <v>4</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="53" spans="5:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E53" s="3">
+        <v>43798</v>
+      </c>
+      <c r="F53" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="G53" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="54" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E54" s="3">
+        <v>43801</v>
+      </c>
+      <c r="F54" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E55" s="3">
+        <v>43805</v>
+      </c>
+      <c r="F55" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked on stream UI - modified hovered menu entries effects - implemented ResourceBundles, first tests
</commit_message>
<xml_diff>
--- a/docs/Arbeitszeit_Topeiner.xlsx
+++ b/docs/Arbeitszeit_Topeiner.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DiplomarbeitFileSharing\stream\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8A74F5-8886-4B99-95FB-0B0EC723848F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91281B36-C42C-4AE1-ADDB-C070CCE36A43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
   <si>
     <t>Arbeitszeit Topeiner</t>
   </si>
@@ -168,6 +168,11 @@
   <si>
     <t>Team-Meeting mit Betreuungslehrer, Noch ausstehende Funktionen überdacht und ausgemacht
 (--&gt; resizeable, FileChooser, ResourceBundles, …)</t>
+  </si>
+  <si>
+    <t>Anpassungen der Effekte beim Bewegen über Menüpunkte
+Recherche und Erstimplementierung von ResourceBundles
+Codedokumentierung</t>
   </si>
 </sst>
 </file>
@@ -559,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B46" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" topLeftCell="B38" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -604,7 +609,7 @@
       </c>
       <c r="C5" s="8">
         <f>SUM(F:F)</f>
-        <v>72.45</v>
+        <v>77.95</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1144,6 +1149,17 @@
       </c>
       <c r="G55" s="5" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="56" spans="5:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E56" s="3">
+        <v>43812</v>
+      </c>
+      <c r="F56" s="4">
+        <v>5.5</v>
+      </c>
+      <c r="G56" s="9" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked on stream UI - added some additional tables - fixed bug which occured while using Table Views
</commit_message>
<xml_diff>
--- a/docs/Arbeitszeit_Topeiner.xlsx
+++ b/docs/Arbeitszeit_Topeiner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DiplomarbeitFileSharing\stream\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91281B36-C42C-4AE1-ADDB-C070CCE36A43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B7064F3-7C20-4CA8-9285-F9CB6FF11513}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
   <si>
     <t>Arbeitszeit Topeiner</t>
   </si>
@@ -173,6 +173,20 @@
     <t>Anpassungen der Effekte beim Bewegen über Menüpunkte
 Recherche und Erstimplementierung von ResourceBundles
 Codedokumentierung</t>
+  </si>
+  <si>
+    <t>Recherche zum Theme java preferences</t>
+  </si>
+  <si>
+    <t>Testen und Erstimplementierung von java preferences</t>
+  </si>
+  <si>
+    <t>Statusupdate erstellt
+Änderungen an stream UI vorgenommen, die durch die Zusammenführung mit dem Backend notwendig waren</t>
+  </si>
+  <si>
+    <t>Zusätzliche Tabellen für die Anzeige von diversen Torrents erstellt
+Bug behoben, bei dem Einträge in Tabellen nicht angezeigt bzw. nicht auswählbar waren</t>
   </si>
 </sst>
 </file>
@@ -564,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B38" workbookViewId="0">
-      <selection activeCell="G59" sqref="G59"/>
+    <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
+      <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -609,7 +623,7 @@
       </c>
       <c r="C5" s="8">
         <f>SUM(F:F)</f>
-        <v>77.95</v>
+        <v>89.7</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1160,6 +1174,72 @@
       </c>
       <c r="G56" s="9" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="57" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E57" s="3">
+        <v>43815</v>
+      </c>
+      <c r="F57" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E58" s="3">
+        <v>43816</v>
+      </c>
+      <c r="F58" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="59" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E59" s="3">
+        <v>43821</v>
+      </c>
+      <c r="F59" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="60" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E60" s="3">
+        <v>43825</v>
+      </c>
+      <c r="F60" s="4">
+        <v>3</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="61" spans="5:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E61" s="3">
+        <v>43829</v>
+      </c>
+      <c r="F61" s="4">
+        <v>2</v>
+      </c>
+      <c r="G61" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="62" spans="5:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E62" s="3">
+        <v>43802</v>
+      </c>
+      <c r="F62" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="G62" s="9" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked on stream UI - modified .properties files - replaced 2 checkboxes with radio buttons
</commit_message>
<xml_diff>
--- a/docs/Arbeitszeit_Topeiner.xlsx
+++ b/docs/Arbeitszeit_Topeiner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DiplomarbeitFileSharing\stream\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B7064F3-7C20-4CA8-9285-F9CB6FF11513}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1285FEA-5001-49D9-8E1A-8E5D9F709294}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
   <si>
     <t>Arbeitszeit Topeiner</t>
   </si>
@@ -187,6 +187,17 @@
   <si>
     <t>Zusätzliche Tabellen für die Anzeige von diversen Torrents erstellt
 Bug behoben, bei dem Einträge in Tabellen nicht angezeigt bzw. nicht auswählbar waren</t>
+  </si>
+  <si>
+    <t>Implementierung von Resource Bundles in die Applikation abgeschlossen
+.properties files mit weiteren Einträgen ergänzt
+Bug behoben, bei dem sich die Position der Menüeinträge beim Ändern der Sprache geändert hat
+Speicherung der Daten in java preferences umgesetzt
+Anpassungen an UI vorgenommen</t>
+  </si>
+  <si>
+    <t>Ersetzen von 2 checkboxes durch radio buttons
+Anpassungen an UI vorgenommen</t>
   </si>
 </sst>
 </file>
@@ -578,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
-      <selection activeCell="G64" sqref="G64"/>
+    <sheetView tabSelected="1" topLeftCell="B55" workbookViewId="0">
+      <selection activeCell="G65" sqref="G64:G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -623,7 +634,7 @@
       </c>
       <c r="C5" s="8">
         <f>SUM(F:F)</f>
-        <v>89.7</v>
+        <v>97.7</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1240,6 +1251,28 @@
       </c>
       <c r="G62" s="9" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="63" spans="5:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="E63" s="3">
+        <v>43835</v>
+      </c>
+      <c r="F63" s="4">
+        <v>6</v>
+      </c>
+      <c r="G63" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="64" spans="5:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E64" s="3">
+        <v>43836</v>
+      </c>
+      <c r="F64" s="4">
+        <v>2</v>
+      </c>
+      <c r="G64" s="9" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked on stream UI - modified .properties files - added animations for some buttons if mouse enters the button
</commit_message>
<xml_diff>
--- a/docs/Arbeitszeit_Topeiner.xlsx
+++ b/docs/Arbeitszeit_Topeiner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DiplomarbeitFileSharing\stream\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1285FEA-5001-49D9-8E1A-8E5D9F709294}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B243BF-698F-47EC-96A8-3102507FFC83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
   <si>
     <t>Arbeitszeit Topeiner</t>
   </si>
@@ -198,6 +198,10 @@
   <si>
     <t>Ersetzen von 2 checkboxes durch radio buttons
 Anpassungen an UI vorgenommen</t>
+  </si>
+  <si>
+    <t>Einfügen von Animationen beim Bewegen der Maus über einige Buttons
+Ergänzungen der ResourceBundle Dateien</t>
   </si>
 </sst>
 </file>
@@ -589,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B55" workbookViewId="0">
-      <selection activeCell="G65" sqref="G64:G65"/>
+    <sheetView tabSelected="1" topLeftCell="B64" workbookViewId="0">
+      <selection activeCell="G66" sqref="G66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -634,7 +638,7 @@
       </c>
       <c r="C5" s="8">
         <f>SUM(F:F)</f>
-        <v>97.7</v>
+        <v>99.2</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1273,6 +1277,17 @@
       </c>
       <c r="G64" s="9" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="65" spans="5:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E65" s="3">
+        <v>43837</v>
+      </c>
+      <c r="F65" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="G65" s="9" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- worked on stream UI - modified application for 'Tag der offenen Tür'
</commit_message>
<xml_diff>
--- a/docs/Arbeitszeit_Topeiner.xlsx
+++ b/docs/Arbeitszeit_Topeiner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DiplomarbeitFileSharing\stream\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B243BF-698F-47EC-96A8-3102507FFC83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922CDB41-11E1-433E-AA21-5F1840906737}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
   <si>
     <t>Arbeitszeit Topeiner</t>
   </si>
@@ -201,7 +201,14 @@
   </si>
   <si>
     <t>Einfügen von Animationen beim Bewegen der Maus über einige Buttons
-Ergänzungen der ResourceBundle Dateien</t>
+Ergänzungen der ResourceBundle Dateien
+Bug gefixed, bei dem Auswählen des default download directories nicht mehr möglich war (Fehler im Umgang mit preferences)
+readme.md aktualisiert</t>
+  </si>
+  <si>
+    <t>Codedokumentierung
+Anpassungen für TdOT (Einfügen neuer Seite, Counter bis Release)
+Diverse Vorbereitungen für TdOT getroffen</t>
   </si>
 </sst>
 </file>
@@ -593,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B64" workbookViewId="0">
-      <selection activeCell="G66" sqref="G66"/>
+    <sheetView tabSelected="1" topLeftCell="B61" workbookViewId="0">
+      <selection activeCell="G68" sqref="G66:G68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -638,7 +645,7 @@
       </c>
       <c r="C5" s="8">
         <f>SUM(F:F)</f>
-        <v>99.2</v>
+        <v>106.7</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1279,15 +1286,26 @@
         <v>51</v>
       </c>
     </row>
-    <row r="65" spans="5:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="65" spans="5:7" ht="72" x14ac:dyDescent="0.3">
       <c r="E65" s="3">
         <v>43837</v>
       </c>
       <c r="F65" s="4">
-        <v>1.5</v>
+        <v>5</v>
       </c>
       <c r="G65" s="9" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="66" spans="5:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E66" s="3">
+        <v>43840</v>
+      </c>
+      <c r="F66" s="4">
+        <v>4</v>
+      </c>
+      <c r="G66" s="9" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- modified menu 'About'
</commit_message>
<xml_diff>
--- a/docs/Arbeitszeit_Topeiner.xlsx
+++ b/docs/Arbeitszeit_Topeiner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DiplomarbeitFileSharing\stream\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922CDB41-11E1-433E-AA21-5F1840906737}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E56080A-6705-41D8-87B3-C9272E75B6AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="55">
   <si>
     <t>Arbeitszeit Topeiner</t>
   </si>
@@ -209,6 +209,9 @@
     <t>Codedokumentierung
 Anpassungen für TdOT (Einfügen neuer Seite, Counter bis Release)
 Diverse Vorbereitungen für TdOT getroffen</t>
+  </si>
+  <si>
+    <t>Live-Bearbeitung und Demos von Projekt</t>
   </si>
 </sst>
 </file>
@@ -600,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G66"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B61" workbookViewId="0">
-      <selection activeCell="G68" sqref="G66:G68"/>
+      <selection activeCell="G68" sqref="G68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -645,7 +648,7 @@
       </c>
       <c r="C5" s="8">
         <f>SUM(F:F)</f>
-        <v>106.7</v>
+        <v>112.7</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1306,6 +1309,17 @@
       </c>
       <c r="G66" s="9" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="67" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E67" s="3">
+        <v>43841</v>
+      </c>
+      <c r="F67" s="4">
+        <v>6</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- optimized stream ui for languages French and Spanish - added some documentation for several functions - modified several ResourceBundles
</commit_message>
<xml_diff>
--- a/docs/Arbeitszeit_Topeiner.xlsx
+++ b/docs/Arbeitszeit_Topeiner.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DiplomarbeitFileSharing\stream\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E56080A-6705-41D8-87B3-C9272E75B6AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CBD541-F78E-4300-A5D1-224478E63580}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
   <si>
     <t>Arbeitszeit Topeiner</t>
   </si>
@@ -212,6 +212,12 @@
   </si>
   <si>
     <t>Live-Bearbeitung und Demos von Projekt</t>
+  </si>
+  <si>
+    <t>Darstellung von allgemeinen Informationen über stream im Menüpunkt 'About'</t>
+  </si>
+  <si>
+    <t>Implementieren 2 neuer Sprachen (Französisch und Spanisch) durch ResourceBundles</t>
   </si>
 </sst>
 </file>
@@ -603,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G67"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B61" workbookViewId="0">
-      <selection activeCell="G68" sqref="G68"/>
+    <sheetView tabSelected="1" topLeftCell="B64" workbookViewId="0">
+      <selection activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -648,7 +654,7 @@
       </c>
       <c r="C5" s="8">
         <f>SUM(F:F)</f>
-        <v>112.7</v>
+        <v>118.7</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1302,7 +1308,7 @@
     </row>
     <row r="66" spans="5:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="E66" s="3">
-        <v>43840</v>
+        <v>43839</v>
       </c>
       <c r="F66" s="4">
         <v>4</v>
@@ -1313,13 +1319,35 @@
     </row>
     <row r="67" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E67" s="3">
-        <v>43841</v>
+        <v>43840</v>
       </c>
       <c r="F67" s="4">
         <v>6</v>
       </c>
       <c r="G67" s="5" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="68" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E68" s="3">
+        <v>43841</v>
+      </c>
+      <c r="F68" s="4">
+        <v>5</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="69" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E69" s="3">
+        <v>43842</v>
+      </c>
+      <c r="F69" s="4">
+        <v>1</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- modified stream UI - updated document 'Arbeitszeit_Topeiner'
</commit_message>
<xml_diff>
--- a/docs/Arbeitszeit_Topeiner.xlsx
+++ b/docs/Arbeitszeit_Topeiner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DiplomarbeitFileSharing\stream\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CBD541-F78E-4300-A5D1-224478E63580}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB62A376-F995-4791-BD94-FC977F5C1306}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="58">
   <si>
     <t>Arbeitszeit Topeiner</t>
   </si>
@@ -218,6 +218,11 @@
   </si>
   <si>
     <t>Implementieren 2 neuer Sprachen (Französisch und Spanisch) durch ResourceBundles</t>
+  </si>
+  <si>
+    <t>Optimierung der stream UI für die neu implementierten Sprachen Französisch und Spanisch
+Ergänzungen der ResourceBundles
+Dokumentation der noch ausstehenden Funktionen</t>
   </si>
 </sst>
 </file>
@@ -609,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G69"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B64" workbookViewId="0">
-      <selection activeCell="E70" sqref="E70"/>
+      <selection activeCell="G70" sqref="G70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -654,7 +659,7 @@
       </c>
       <c r="C5" s="8">
         <f>SUM(F:F)</f>
-        <v>118.7</v>
+        <v>120.7</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1348,6 +1353,17 @@
       </c>
       <c r="G69" s="5" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="70" spans="5:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E70" s="3">
+        <v>43843</v>
+      </c>
+      <c r="F70" s="4">
+        <v>2</v>
+      </c>
+      <c r="G70" s="9" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented css files to project
</commit_message>
<xml_diff>
--- a/docs/Arbeitszeit_Topeiner.xlsx
+++ b/docs/Arbeitszeit_Topeiner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DiplomarbeitFileSharing\stream\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB62A376-F995-4791-BD94-FC977F5C1306}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC2B497-E9EF-4F73-A08A-30D2D42221E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="59">
   <si>
     <t>Arbeitszeit Topeiner</t>
   </si>
@@ -206,11 +206,6 @@
 readme.md aktualisiert</t>
   </si>
   <si>
-    <t>Codedokumentierung
-Anpassungen für TdOT (Einfügen neuer Seite, Counter bis Release)
-Diverse Vorbereitungen für TdOT getroffen</t>
-  </si>
-  <si>
     <t>Live-Bearbeitung und Demos von Projekt</t>
   </si>
   <si>
@@ -222,7 +217,19 @@
   <si>
     <t>Optimierung der stream UI für die neu implementierten Sprachen Französisch und Spanisch
 Ergänzungen der ResourceBundles
-Dokumentation der noch ausstehenden Funktionen</t>
+Dokumentation der noch ausstehenden Funktionen
+Kurzes Teammeeting
+Statusupdate erstellt</t>
+  </si>
+  <si>
+    <t>Codedokumentierung
+Anpassungen für TdOT (Einfügen neuer Seite 'Über', Counter bis Release)
+Diverse Vorbereitungen für TdOT getroffen</t>
+  </si>
+  <si>
+    <t>Arbeiten an stream App Icon
+Einführung von css files (Notwendig durch die zukünftige Implementierung eines Dark modes)
+Annpassungen an stream UI wegen Einführung von css files</t>
   </si>
 </sst>
 </file>
@@ -614,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G70"/>
+  <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B64" workbookViewId="0">
-      <selection activeCell="G70" sqref="G70"/>
+      <selection activeCell="F69" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -659,7 +666,7 @@
       </c>
       <c r="C5" s="8">
         <f>SUM(F:F)</f>
-        <v>120.7</v>
+        <v>129.19999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1319,7 +1326,7 @@
         <v>4</v>
       </c>
       <c r="G66" s="9" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="67" spans="5:7" x14ac:dyDescent="0.3">
@@ -1330,7 +1337,7 @@
         <v>6</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="68" spans="5:7" x14ac:dyDescent="0.3">
@@ -1341,7 +1348,7 @@
         <v>5</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="69" spans="5:7" x14ac:dyDescent="0.3">
@@ -1352,18 +1359,29 @@
         <v>1</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="70" spans="5:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="70" spans="5:7" ht="72" x14ac:dyDescent="0.3">
       <c r="E70" s="3">
         <v>43843</v>
       </c>
       <c r="F70" s="4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G70" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="71" spans="5:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E71" s="3">
+        <v>43844</v>
+      </c>
+      <c r="F71" s="4">
+        <v>5.5</v>
+      </c>
+      <c r="G71" s="9" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed bug concerning dark mode
</commit_message>
<xml_diff>
--- a/docs/Arbeitszeit_Topeiner.xlsx
+++ b/docs/Arbeitszeit_Topeiner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DiplomarbeitFileSharing\stream\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF9777DF-BF48-4EDB-90CC-25639C9C877A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1B2EC0-90F6-4E33-B1D5-BF17227EEC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="62">
   <si>
     <t>Arbeitszeit Topeiner</t>
   </si>
@@ -631,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G74"/>
+  <dimension ref="A1:G75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B70" workbookViewId="0">
-      <selection activeCell="G79" sqref="G78:G79"/>
+      <selection activeCell="G76" sqref="G76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -676,7 +676,7 @@
       </c>
       <c r="C5" s="8">
         <f>SUM(F:F)</f>
-        <v>137.19999999999999</v>
+        <v>138.19999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1425,6 +1425,17 @@
       </c>
       <c r="G74" s="9" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="75" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E75" s="3">
+        <v>43857</v>
+      </c>
+      <c r="F75" s="4">
+        <v>1</v>
+      </c>
+      <c r="G75" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>